<commit_message>
Formatos condicionales, parte 2
</commit_message>
<xml_diff>
--- a/Excel/Práctica/17. Formatos condicionales en Excel/Escalas de color, para hacer la información mucho más visual al comparar cantidades de menor a mayor.xlsx
+++ b/Excel/Práctica/17. Formatos condicionales en Excel/Escalas de color, para hacer la información mucho más visual al comparar cantidades de menor a mayor.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="542">
   <si>
     <t>NO 
 EMPLEADO</t>
@@ -1871,43 +1871,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Ahora, también podemos personalizar los formatos condicionales; es decir, especificar por nuestra propia cuenta qué juego de colores queremos asignar sobre estos registros numéricos y/o metricas según unas condiciones que pasemos (y que se deben cumplir) sobre ellos. Por ejemplo, si quisieramos que se aplique un formato condicional, en particular, sobre todos los registros que sean mayor a mil (&gt; 1000) en la columna </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Precio Venta Producto...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">lo podemos hacer; tenemos total libertad de elegir con qué color destacar estos tipos de registros en especifico. Este recurso se encuentra en la opción </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Resaltar reglas de celdas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">También puede determinar sobre qué campos eliminar los formatos condicionales ya establecidos previamente, eso se hace en la opción </t>
     </r>
     <r>
@@ -1943,13 +1906,118 @@
       <t>Formato condicional.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ahora, también podemos personalizar los formatos condicionales; es decir, especificar por nuestra propia cuenta qué juego de colores queremos asignar sobre estos registros numéricos y/o metricas según unas condiciones que pasemos (y que se deben cumplir) sobre ellos. Por ejemplo, si quisieramos que se aplique un formato condicional, en particular, sobre todos los registros que sean mayor a mil (&gt; 1000) en la columna </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Precio Venta Producto...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lo podemos hacer; tenemos total libertad de elegir con qué color destacar estos tipos de registros en especifico. Este recurso del ejemplo se encuentra en la opción </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resaltar reglas de celdas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Todas las reglas que hayamos creados son modificables, esto se hace dentro de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Administrar reglas… </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Al igual, desde aquí mismo, tiene la libertad de elegir que regla eliminar, una a una y a voluntad propia.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ahora, en la opción </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nueva regla... </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">podemos personalizar aún más todas las reglas; es decir, los parámetros válidos, para identificar con estos formatos de colores, nuestros resultados numéricos; esto, lo dicho, según unas condiciones pasadas que, inclusive, pueden ser definidas por nosotros mismos ... haciendo uso hasta de condicionales (he aquí la parte recursiva de la herramienta al dejarnos personalizar los formatos condicionales a nuestro gusto). Revise todas las opciones del estilo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clásico...</t>
+    </r>
+  </si>
+  <si>
+    <t>Revise el siguiente caso (corresponde a los formatos condicionales pasados a nuestra primera columna)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -2127,15 +2195,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
@@ -2151,21 +2220,43 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Énfasis1" xfId="5" builtinId="29"/>
     <cellStyle name="EstiloNaraja" xfId="1"/>
     <cellStyle name="Moneda" xfId="4" builtinId="4"/>
+    <cellStyle name="Moneda [0]" xfId="6" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2178,11 +2269,291 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2207,6 +2578,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>233826</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9347200" y="9652000"/>
+          <a:ext cx="5105400" cy="2405526"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9347200" y="13512800"/>
+          <a:ext cx="6388100" cy="2717800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2508,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:O31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2545,7 +3009,7 @@
       <c r="A2" t="s">
         <v>467</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="12">
         <v>100</v>
       </c>
       <c r="C2">
@@ -2567,7 +3031,7 @@
       <c r="A3" t="s">
         <v>468</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <v>200</v>
       </c>
       <c r="C3">
@@ -2584,22 +3048,22 @@
         <f t="shared" ref="F3:F63" si="1">C3*E3</f>
         <v>15000</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>536</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>469</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="12">
         <v>300</v>
       </c>
       <c r="C4">
@@ -2616,20 +3080,20 @@
         <f t="shared" si="1"/>
         <v>930000</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>470</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="12">
         <v>1000</v>
       </c>
       <c r="C5">
@@ -2646,20 +3110,20 @@
         <f t="shared" si="1"/>
         <v>400000</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>471</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="12">
         <v>900</v>
       </c>
       <c r="C6">
@@ -2676,20 +3140,20 @@
         <f t="shared" si="1"/>
         <v>90000</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>472</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="12">
         <v>200</v>
       </c>
       <c r="C7">
@@ -2706,20 +3170,20 @@
         <f t="shared" si="1"/>
         <v>90000</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>473</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="12">
         <v>300</v>
       </c>
       <c r="C8">
@@ -2736,20 +3200,20 @@
         <f t="shared" si="1"/>
         <v>120000</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>474</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="12">
         <v>100</v>
       </c>
       <c r="C9">
@@ -2766,19 +3230,19 @@
         <f t="shared" si="1"/>
         <v>27000</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>475</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="12">
         <v>80</v>
       </c>
       <c r="C10">
@@ -2795,22 +3259,22 @@
         <f t="shared" si="1"/>
         <v>88000</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="11" t="s">
         <v>534</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>476</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="12">
         <v>70</v>
       </c>
       <c r="C11">
@@ -2827,20 +3291,20 @@
         <f t="shared" si="1"/>
         <v>14000</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>477</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="12">
         <v>1000</v>
       </c>
       <c r="C12">
@@ -2857,20 +3321,20 @@
         <f t="shared" si="1"/>
         <v>800000</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>478</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="12">
         <v>100</v>
       </c>
       <c r="C13">
@@ -2887,20 +3351,20 @@
         <f t="shared" si="1"/>
         <v>11000</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>479</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="12">
         <v>300</v>
       </c>
       <c r="C14">
@@ -2917,20 +3381,20 @@
         <f t="shared" si="1"/>
         <v>224000</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
     </row>
     <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>480</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="12">
         <v>400</v>
       </c>
       <c r="C15">
@@ -2947,20 +3411,20 @@
         <f t="shared" si="1"/>
         <v>330000</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>481</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="12">
         <v>900</v>
       </c>
       <c r="C16">
@@ -2977,20 +3441,20 @@
         <f t="shared" si="1"/>
         <v>50000</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>482</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="12">
         <v>100</v>
       </c>
       <c r="C17">
@@ -3012,7 +3476,7 @@
       <c r="A18" t="s">
         <v>483</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="12">
         <v>100</v>
       </c>
       <c r="C18">
@@ -3029,22 +3493,22 @@
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>484</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="12">
         <v>200</v>
       </c>
       <c r="C19">
@@ -3061,20 +3525,20 @@
         <f t="shared" si="1"/>
         <v>24000</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>485</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="12">
         <v>300</v>
       </c>
       <c r="C20">
@@ -3091,20 +3555,20 @@
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>486</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="12">
         <v>1000</v>
       </c>
       <c r="C21">
@@ -3126,7 +3590,7 @@
       <c r="A22" t="s">
         <v>487</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="12">
         <v>900</v>
       </c>
       <c r="C22">
@@ -3143,22 +3607,22 @@
         <f t="shared" si="1"/>
         <v>720000</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+      <c r="H22" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>488</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="12">
         <v>200</v>
       </c>
       <c r="C23">
@@ -3175,20 +3639,20 @@
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>489</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="12">
         <v>300</v>
       </c>
       <c r="C24">
@@ -3205,20 +3669,20 @@
         <f t="shared" si="1"/>
         <v>88000</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>490</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="12">
         <v>100</v>
       </c>
       <c r="C25">
@@ -3235,20 +3699,20 @@
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>491</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="12">
         <v>80</v>
       </c>
       <c r="C26">
@@ -3265,20 +3729,20 @@
         <f t="shared" si="1"/>
         <v>28000</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>492</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="12">
         <v>70</v>
       </c>
       <c r="C27">
@@ -3295,20 +3759,20 @@
         <f t="shared" si="1"/>
         <v>39000</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>493</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="12">
         <v>1000</v>
       </c>
       <c r="C28">
@@ -3325,20 +3789,20 @@
         <f t="shared" si="1"/>
         <v>800000</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>494</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="12">
         <v>100</v>
       </c>
       <c r="C29">
@@ -3360,7 +3824,7 @@
       <c r="A30" t="s">
         <v>495</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="12">
         <v>300</v>
       </c>
       <c r="C30">
@@ -3377,22 +3841,22 @@
         <f t="shared" si="1"/>
         <v>330000</v>
       </c>
-      <c r="H30" s="10" t="s">
-        <v>538</v>
-      </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
+      <c r="H30" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>496</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="12">
         <v>400</v>
       </c>
       <c r="C31">
@@ -3409,20 +3873,20 @@
         <f t="shared" si="1"/>
         <v>80000</v>
       </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
     </row>
     <row r="32" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>497</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="12">
         <v>900</v>
       </c>
       <c r="C32">
@@ -3440,11 +3904,11 @@
         <v>420000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>498</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="12">
         <v>100</v>
       </c>
       <c r="C33">
@@ -3461,12 +3925,22 @@
         <f t="shared" si="1"/>
         <v>90000</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+    </row>
+    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>499</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="12">
         <v>100</v>
       </c>
       <c r="C34">
@@ -3483,12 +3957,20 @@
         <f t="shared" si="1"/>
         <v>96000</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+    </row>
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>500</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="12">
         <v>200</v>
       </c>
       <c r="C35">
@@ -3505,12 +3987,20 @@
         <f t="shared" si="1"/>
         <v>7000</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+    </row>
+    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>501</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="12">
         <v>300</v>
       </c>
       <c r="C36">
@@ -3527,12 +4017,20 @@
         <f t="shared" si="1"/>
         <v>120000</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+    </row>
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>502</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="12">
         <v>1000</v>
       </c>
       <c r="C37">
@@ -3549,12 +4047,20 @@
         <f t="shared" si="1"/>
         <v>8000</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+    </row>
+    <row r="38" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>503</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="12">
         <v>900</v>
       </c>
       <c r="C38">
@@ -3572,11 +4078,11 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>504</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="12">
         <v>200</v>
       </c>
       <c r="C39">
@@ -3594,11 +4100,11 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>505</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="12">
         <v>300</v>
       </c>
       <c r="C40">
@@ -3616,11 +4122,11 @@
         <v>140000</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>506</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="12">
         <v>100</v>
       </c>
       <c r="C41">
@@ -3638,11 +4144,11 @@
         <v>72000</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>507</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="12">
         <v>80</v>
       </c>
       <c r="C42">
@@ -3660,11 +4166,11 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>508</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="12">
         <v>70</v>
       </c>
       <c r="C43">
@@ -3682,11 +4188,11 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>509</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="12">
         <v>1000</v>
       </c>
       <c r="C44">
@@ -3704,11 +4210,11 @@
         <v>440000</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>510</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="12">
         <v>100</v>
       </c>
       <c r="C45">
@@ -3726,11 +4232,11 @@
         <v>117000</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>511</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="12">
         <v>300</v>
       </c>
       <c r="C46">
@@ -3748,11 +4254,11 @@
         <v>88000</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>512</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="12">
         <v>400</v>
       </c>
       <c r="C47">
@@ -3770,11 +4276,11 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>513</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="12">
         <v>900</v>
       </c>
       <c r="C48">
@@ -3796,7 +4302,7 @@
       <c r="A49" t="s">
         <v>514</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="12">
         <v>100</v>
       </c>
       <c r="C49">
@@ -3818,7 +4324,7 @@
       <c r="A50" t="s">
         <v>515</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="12">
         <v>100</v>
       </c>
       <c r="C50">
@@ -3835,12 +4341,22 @@
         <f t="shared" si="1"/>
         <v>30000</v>
       </c>
+      <c r="H50" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
     </row>
     <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>516</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="12">
         <v>200</v>
       </c>
       <c r="C51">
@@ -3857,12 +4373,20 @@
         <f t="shared" si="1"/>
         <v>33000</v>
       </c>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
     </row>
     <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>517</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="12">
         <v>300</v>
       </c>
       <c r="C52">
@@ -3884,7 +4408,7 @@
       <c r="A53" t="s">
         <v>518</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="12">
         <v>1000</v>
       </c>
       <c r="C53">
@@ -3901,12 +4425,22 @@
         <f t="shared" si="1"/>
         <v>750000</v>
       </c>
+      <c r="H53" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
     </row>
     <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>519</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="12">
         <v>900</v>
       </c>
       <c r="C54">
@@ -3928,7 +4462,7 @@
       <c r="A55" t="s">
         <v>520</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="12">
         <v>200</v>
       </c>
       <c r="C55">
@@ -3950,7 +4484,7 @@
       <c r="A56" t="s">
         <v>521</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="12">
         <v>300</v>
       </c>
       <c r="C56">
@@ -3972,7 +4506,7 @@
       <c r="A57" t="s">
         <v>522</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="12">
         <v>100</v>
       </c>
       <c r="C57">
@@ -3994,7 +4528,7 @@
       <c r="A58" t="s">
         <v>523</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="12">
         <v>80</v>
       </c>
       <c r="C58">
@@ -4016,7 +4550,7 @@
       <c r="A59" t="s">
         <v>524</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="12">
         <v>70</v>
       </c>
       <c r="C59">
@@ -4038,7 +4572,7 @@
       <c r="A60" t="s">
         <v>525</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="12">
         <v>1000</v>
       </c>
       <c r="C60">
@@ -4060,7 +4594,7 @@
       <c r="A61" t="s">
         <v>526</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="12">
         <v>100</v>
       </c>
       <c r="C61">
@@ -4082,7 +4616,7 @@
       <c r="A62" t="s">
         <v>527</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="12">
         <v>300</v>
       </c>
       <c r="C62">
@@ -4104,7 +4638,7 @@
       <c r="A63" t="s">
         <v>528</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="12">
         <v>400</v>
       </c>
       <c r="C63">
@@ -4131,7 +4665,10 @@
       <c r="O63"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="H33:O37"/>
+    <mergeCell ref="H50:O51"/>
+    <mergeCell ref="H53:O53"/>
     <mergeCell ref="H22:O28"/>
     <mergeCell ref="H30:O31"/>
     <mergeCell ref="H3:O8"/>
@@ -4140,7 +4677,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4152,7 +4689,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="7">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -4161,7 +4698,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4175,12 +4712,21 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E63">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+      <formula>1000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33">
+    <cfRule type="top10" dxfId="4" priority="3" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B63">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>